<commit_message>
Added entire run perf graph
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>711</v>
+        <v>625</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -474,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>504</v>
+        <v>376</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -490,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>606</v>
+        <v>518</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>668</v>
+        <v>558</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -538,7 +538,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>646</v>
+        <v>398</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -554,7 +554,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>718</v>
+        <v>364</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -570,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>428</v>
+        <v>504</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>678</v>
+        <v>684</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -618,9 +618,857 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>666</v>
       </c>
       <c r="D12" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>546</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="n">
+        <v>546</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="n">
+        <v>316</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>514</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>784</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="n">
+        <v>792</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>742</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="n">
+        <v>974</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1046</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="n">
+        <v>840</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="n">
+        <v>868</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1318</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1164</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1382</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1366</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1146</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1730</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="n">
+        <v>824</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2184</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1462</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1746</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1336</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1112</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" t="n">
+        <v>938</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" t="n">
+        <v>2184</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1664</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1802</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1574</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1438</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>41</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2708</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>42</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2046</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>43</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2328</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>44</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2494</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>45</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1854</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>46</v>
+      </c>
+      <c r="C47" t="n">
+        <v>904</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>47</v>
+      </c>
+      <c r="C48" t="n">
+        <v>658</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>48</v>
+      </c>
+      <c r="C49" t="n">
+        <v>2118</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>49</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1086</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1286</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>51</v>
+      </c>
+      <c r="C52" t="n">
+        <v>2664</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>52</v>
+      </c>
+      <c r="C53" t="n">
+        <v>2022</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>53</v>
+      </c>
+      <c r="C54" t="n">
+        <v>2616</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>54</v>
+      </c>
+      <c r="C55" t="n">
+        <v>2660</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>55</v>
+      </c>
+      <c r="C56" t="n">
+        <v>3730</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>56</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2690</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>57</v>
+      </c>
+      <c r="C58" t="n">
+        <v>3368</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>58</v>
+      </c>
+      <c r="C59" t="n">
+        <v>2830</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>59</v>
+      </c>
+      <c r="C60" t="n">
+        <v>2952</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>60</v>
+      </c>
+      <c r="C61" t="n">
+        <v>2416</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>61</v>
+      </c>
+      <c r="C62" t="n">
+        <v>2340</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>62</v>
+      </c>
+      <c r="C63" t="n">
+        <v>3972</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>63</v>
+      </c>
+      <c r="C64" t="n">
+        <v>3820</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>64</v>
+      </c>
+      <c r="C65" t="n">
+        <v>4373</v>
+      </c>
+      <c r="D65" t="inlineStr">
         <is>
           <t>False</t>
         </is>

</xml_diff>

<commit_message>
Output ep2 and ep3 of 4th expm
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>581</v>
+        <v>782</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -474,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>526</v>
+        <v>486</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -490,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>596</v>
+        <v>642</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -506,7 +506,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>518</v>
+        <v>380</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -522,7 +522,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>698</v>
+        <v>576</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -538,7 +538,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>758</v>
+        <v>348</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -554,7 +554,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>724</v>
+        <v>496</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -570,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -586,7 +586,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>654</v>
+        <v>614</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -602,7 +602,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>652</v>
+        <v>846</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -618,9 +618,25 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>549</v>
+        <v>748</v>
       </c>
       <c r="D12" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>346</v>
+      </c>
+      <c r="D13" t="inlineStr">
         <is>
           <t>False</t>
         </is>

</xml_diff>